<commit_message>
All config tests working, added failing tests to be editied
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="40">
   <si>
     <t>X</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>W = Walkway</t>
+  </si>
+  <si>
+    <t>Number of Doors: 16</t>
+  </si>
+  <si>
+    <t>Blue: door direction tests</t>
   </si>
 </sst>
 </file>
@@ -193,12 +199,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -213,7 +234,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -229,6 +250,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Closet" xfId="1"/>
@@ -534,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +589,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2414,7 +2436,7 @@
       <c r="Q23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="R23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S23" s="2" t="s">
@@ -2677,6 +2699,16 @@
       </c>
       <c r="Y26">
         <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated (MIKE) the ClueGame (put it onto my own computer) and updated Layout for Git Board Part 2 assignment test cells in layout grid
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18195" windowHeight="7995"/>
+    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="48">
   <si>
     <t>X</t>
   </si>
@@ -135,14 +140,38 @@
     <t>Number of Doors: 16</t>
   </si>
   <si>
-    <t>Blue: door direction tests</t>
+    <t>Purple:Locations that are doorways</t>
+  </si>
+  <si>
+    <t>Brown: Locations that have only walkways as adjacent locations</t>
+  </si>
+  <si>
+    <t>Orange: Locations at edge of board</t>
+  </si>
+  <si>
+    <t>Dark Green Locations that are beside a room cell that is not a doorway</t>
+  </si>
+  <si>
+    <t>White: Target Tests for Walkways</t>
+  </si>
+  <si>
+    <t>Army Green: Locations that are next to doorway with needed direction</t>
+  </si>
+  <si>
+    <t>Light Green: Target tests for Rooms</t>
+  </si>
+  <si>
+    <t>TARGET TESTS</t>
+  </si>
+  <si>
+    <t>ADJACENCY TESTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +195,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +250,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF68E930"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -207,23 +295,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0">
@@ -233,8 +306,78 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -250,11 +393,90 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="75">
     <cellStyle name="Closet" xfId="1"/>
     <cellStyle name="Doors" xfId="4"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Room" xfId="2"/>
     <cellStyle name="Walkway" xfId="3"/>
@@ -556,39 +778,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="5" max="5" width="4.5" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" customWidth="1"/>
-    <col min="13" max="13" width="4.42578125" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" customWidth="1"/>
+    <col min="7" max="8" width="4.33203125" customWidth="1"/>
+    <col min="9" max="10" width="4.5" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" customWidth="1"/>
+    <col min="12" max="13" width="4.5" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="19" width="4.85546875" customWidth="1"/>
-    <col min="20" max="20" width="4.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" customWidth="1"/>
-    <col min="23" max="23" width="4.7109375" customWidth="1"/>
+    <col min="18" max="19" width="4.83203125" customWidth="1"/>
+    <col min="20" max="20" width="4.5" customWidth="1"/>
+    <col min="21" max="21" width="5.5" customWidth="1"/>
+    <col min="22" max="22" width="5.1640625" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" customWidth="1"/>
     <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="5.7109375" customWidth="1"/>
+    <col min="25" max="25" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -604,7 +825,7 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -668,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -732,7 +953,7 @@
       <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
@@ -748,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -764,7 +985,7 @@
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -828,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -841,7 +1062,7 @@
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -908,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -942,7 +1163,7 @@
       <c r="K5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -954,13 +1175,13 @@
       <c r="O5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="12" t="s">
         <v>1</v>
       </c>
       <c r="S5" s="2" t="s">
@@ -988,7 +1209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1068,7 +1289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1087,10 +1308,10 @@
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="G7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -1148,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1228,7 +1449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1259,7 +1480,7 @@
       <c r="J9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -1271,7 +1492,7 @@
       <c r="N9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="P9" s="2" t="s">
@@ -1308,7 +1529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1388,7 +1609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1443,7 +1664,7 @@
       <c r="R11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="S11" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="4" t="s">
@@ -1471,7 +1692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1554,7 +1775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1603,7 +1824,7 @@
       <c r="P13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -1637,14 +1858,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1656,7 +1877,7 @@
       <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1704,7 +1925,7 @@
       <c r="V14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="W14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="X14" s="2" t="s">
@@ -1720,7 +1941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1793,7 +2014,7 @@
       <c r="X15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="Y15" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Z15">
@@ -1803,7 +2024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1886,7 +2107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1941,7 +2162,7 @@
       <c r="R17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S17" s="5" t="s">
+      <c r="S17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="T17" s="4" t="s">
@@ -1969,7 +2190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1997,7 +2218,7 @@
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -2021,7 +2242,7 @@
       <c r="Q18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="R18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="5" t="s">
@@ -2052,7 +2273,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2089,7 +2310,7 @@
       <c r="L19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="14" t="s">
         <v>1</v>
       </c>
       <c r="N19" s="2" t="s">
@@ -2135,8 +2356,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:30">
+      <c r="A20" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2172,7 +2393,7 @@
       <c r="L20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N20" s="4" t="s">
@@ -2218,7 +2439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -2240,7 +2461,7 @@
       <c r="G21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -2301,7 +2522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -2384,7 +2605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2464,7 +2685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -2544,7 +2765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -2566,7 +2787,7 @@
       <c r="G25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="11" t="s">
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -2593,13 +2814,13 @@
       <c r="P25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="2" t="s">
+      <c r="S25" s="12" t="s">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
@@ -2617,14 +2838,14 @@
       <c r="X25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y25" s="2" t="s">
+      <c r="Y25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Z25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2701,19 +2922,64 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:30">
+      <c r="A28" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:30">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2723,9 +2989,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2735,8 +3006,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
.metadata; More important, added in a cell calculator in layout for easier use of making tests
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560"/>
+    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Layout" sheetId="1" r:id="rId1"/>
+    <sheet name="Cell Calculator and Tests" sheetId="2" r:id="rId2"/>
+    <sheet name="Room Legend" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="84">
   <si>
     <t>X</t>
   </si>
@@ -155,9 +155,6 @@
     <t>White: Target Tests for Walkways</t>
   </si>
   <si>
-    <t>Army Green: Locations that are next to doorway with needed direction</t>
-  </si>
-  <si>
     <t>Light Green: Target tests for Rooms</t>
   </si>
   <si>
@@ -165,13 +162,124 @@
   </si>
   <si>
     <t>ADJACENCY TESTS</t>
+  </si>
+  <si>
+    <t>Light Green: Locations that are next to doorway with needed direction</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>M19</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Y15</t>
+  </si>
+  <si>
+    <t>H25</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>G14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K9 </t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>W25</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Col</t>
+  </si>
+  <si>
+    <t>//////</t>
+  </si>
+  <si>
+    <t>CELL CALCULATOR FOR TESTS</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Other Cell Calculator</t>
+  </si>
+  <si>
+    <t>Tester To Make Sure It works</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>TOTAL ROWS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL COLS: </t>
+  </si>
+  <si>
+    <t>///////</t>
+  </si>
+  <si>
+    <t>/////</t>
+  </si>
+  <si>
+    <t>A14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,10 +324,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="0.39994506668294322"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="5" tint="0.39994506668294322"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,12 +390,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -286,8 +406,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -295,8 +427,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0">
@@ -376,8 +588,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -399,12 +612,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="75" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="75" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="75" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="75" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="76">
     <cellStyle name="Closet" xfId="1"/>
     <cellStyle name="Doors" xfId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -479,6 +706,7 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Room" xfId="2"/>
+    <cellStyle name="Style 1" xfId="75"/>
     <cellStyle name="Walkway" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -778,38 +1006,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD37"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:AM37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" customWidth="1"/>
-    <col min="5" max="5" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="8" width="4.33203125" customWidth="1"/>
-    <col min="9" max="10" width="4.5" customWidth="1"/>
-    <col min="11" max="11" width="4.1640625" customWidth="1"/>
-    <col min="12" max="13" width="4.5" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" customWidth="1"/>
-    <col min="16" max="16" width="5.5" customWidth="1"/>
-    <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="19" width="4.83203125" customWidth="1"/>
-    <col min="20" max="20" width="4.5" customWidth="1"/>
-    <col min="21" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="22" width="5.1640625" customWidth="1"/>
-    <col min="23" max="23" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="4.28515625" customWidth="1"/>
+    <col min="9" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+    <col min="12" max="13" width="4.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.85546875" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="5.6640625" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" customWidth="1"/>
+    <col min="26" max="29" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6" customWidth="1"/>
+    <col min="31" max="31" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" customWidth="1"/>
+    <col min="33" max="38" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -825,7 +1059,7 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -889,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -953,7 +1187,7 @@
       <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
@@ -969,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -985,7 +1219,7 @@
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1049,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1062,7 +1296,7 @@
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1129,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1163,7 +1397,7 @@
       <c r="K5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1175,13 +1409,13 @@
       <c r="O5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S5" s="2" t="s">
@@ -1209,7 +1443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1289,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1308,7 +1542,7 @@
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -1369,7 +1603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1480,10 +1714,10 @@
       <c r="J9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="K9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -1492,14 +1726,14 @@
       <c r="N9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>1</v>
@@ -1529,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1609,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1664,7 +1898,7 @@
       <c r="R11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="S11" s="13" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="4" t="s">
@@ -1692,7 +1926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1775,7 +2009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1858,14 +2092,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1877,7 +2111,7 @@
       <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1925,7 +2159,7 @@
       <c r="V14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="12" t="s">
+      <c r="W14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="X14" s="2" t="s">
@@ -1941,7 +2175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2014,7 +2248,7 @@
       <c r="X15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y15" s="10" t="s">
+      <c r="Y15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Z15">
@@ -2024,7 +2258,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2107,7 +2341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2190,7 +2424,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2242,7 +2476,7 @@
       <c r="Q18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="R18" s="13" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="5" t="s">
@@ -2273,7 +2507,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2310,7 +2544,7 @@
       <c r="L19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N19" s="2" t="s">
@@ -2356,8 +2590,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2439,7 +2673,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -2461,7 +2695,7 @@
       <c r="G21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -2522,7 +2756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -2605,7 +2839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2657,7 +2891,7 @@
       <c r="Q23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="R23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S23" s="2" t="s">
@@ -2685,7 +2919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -2737,7 +2971,7 @@
       <c r="Q24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="R24" s="11" t="s">
         <v>1</v>
       </c>
       <c r="S24" s="2" t="s">
@@ -2765,7 +2999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -2787,7 +3021,7 @@
       <c r="G25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -2814,13 +3048,13 @@
       <c r="P25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Q25" s="10" t="s">
+      <c r="Q25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="12" t="s">
+      <c r="S25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
@@ -2832,20 +3066,20 @@
       <c r="V25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="W25" s="11" t="s">
         <v>1</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y25" s="10" t="s">
+      <c r="Y25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="Z25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2920,56 +3154,6 @@
       </c>
       <c r="Y26">
         <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30">
-      <c r="A28" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2985,12 +3169,904 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="14">
+        <f>CODE(LEFT(B3,1)) -64</f>
+        <v>17</v>
+      </c>
+      <c r="D3" s="15" t="str">
+        <f>MID(B3,2,LEN(B3) -1)</f>
+        <v>13</v>
+      </c>
+      <c r="E3" s="16">
+        <f>((D3-1)*25) +(C3)</f>
+        <v>317</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="14">
+        <f>CODE(LEFT(F3,1)) -64</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="15" t="str">
+        <f>MID(F3,2,LEN(F3) -1)</f>
+        <v>18</v>
+      </c>
+      <c r="I3" s="16">
+        <f>((H3-1)*25) +(G3)</f>
+        <v>435</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="15" t="str">
+        <f>MID(J3,2,LEN(J3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="15" t="str">
+        <f>MID(N3,2,LEN(N3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="15" t="str">
+        <f>MID(R3,2,LEN(R3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X3" s="15" t="str">
+        <f>MID(V3,2,LEN(V3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="14">
+        <f t="shared" ref="C4:C10" si="0">CODE(LEFT(B4,1)) -64</f>
+        <v>17</v>
+      </c>
+      <c r="D4" s="15" t="str">
+        <f>MID(B4,2,LEN(B4) -1)</f>
+        <v>25</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" ref="E4:E10" si="1">((D4-1)*25) +(C4)</f>
+        <v>617</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" ref="G4:G10" si="2">CODE(LEFT(F4,1)) -64</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="15" t="str">
+        <f>MID(F4,2,LEN(F4) -1)</f>
+        <v>20</v>
+      </c>
+      <c r="I4" s="16">
+        <f t="shared" ref="I4:I7" si="3">((H4-1)*25) +(G4)</f>
+        <v>476</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" ref="K4:K10" si="4">CODE(LEFT(J4,1)) -64</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="15" t="str">
+        <f>MID(J4,2,LEN(J4) -1)</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="16">
+        <f t="shared" ref="M4:M7" si="5">((L4-1)*25) +(K4)</f>
+        <v>6</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O10" si="6">CODE(LEFT(N4,1)) -64</f>
+        <v>25</v>
+      </c>
+      <c r="P4" s="15" t="str">
+        <f>MID(N4,2,LEN(N4) -1)</f>
+        <v>15</v>
+      </c>
+      <c r="Q4" s="16">
+        <f t="shared" ref="Q4:Q7" si="7">((P4-1)*25) +(O4)</f>
+        <v>375</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T4" s="15" t="str">
+        <f>MID(R4,2,LEN(R4) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X4" s="15" t="str">
+        <f>MID(V4,2,LEN(V4) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D5" s="15" t="str">
+        <f t="shared" ref="D5:D10" si="8">MID(B5,2,LEN(B5) -1)</f>
+        <v>25</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="1"/>
+        <v>608</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H5" s="15" t="str">
+        <f t="shared" ref="H5:H10" si="9">MID(F5,2,LEN(F5) -1)</f>
+        <v>5</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="15" t="str">
+        <f t="shared" ref="L5:L10" si="10">MID(J5,2,LEN(J5) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P5" s="15" t="str">
+        <f t="shared" ref="P5:P10" si="11">MID(N5,2,LEN(N5) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T5" s="15" t="str">
+        <f t="shared" ref="T5:T10" si="12">MID(R5,2,LEN(R5) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5" s="15" t="str">
+        <f t="shared" ref="X5:X10" si="13">MID(V5,2,LEN(V5) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y5" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="H6" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" si="3"/>
+        <v>269</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="L6" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="M6" s="16">
+        <f t="shared" si="5"/>
+        <v>443</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="P6" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="Q6" s="16">
+        <f t="shared" si="7"/>
+        <v>463</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T6" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v>/////</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V6" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X6" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v>/////</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" si="3"/>
+        <v>158</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="L7" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="M7" s="16">
+        <f t="shared" si="5"/>
+        <v>419</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v>/////</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T7" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v>/////</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X7" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v>/////</v>
+      </c>
+      <c r="Y7" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>/////</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>/////</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>/////</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P8" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v>/////</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T8" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v>/////</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="V8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X8" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v>/////</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D9" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="1"/>
+        <v>328</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H9" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" ref="I9:I10" si="14">((H9-1)*25) +(G9)</f>
+        <v>212</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="L9" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="M9" s="16">
+        <f t="shared" ref="M9:M10" si="15">((L9-1)*25) +(K9)</f>
+        <v>593</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="P9" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">9 </v>
+      </c>
+      <c r="Q9" s="16">
+        <f t="shared" ref="Q9:Q10" si="16">((P9-1)*25) +(O9)</f>
+        <v>211</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="S9" s="14">
+        <f t="shared" ref="S4:S10" si="17">CODE(LEFT(R9,1)) -64</f>
+        <v>7</v>
+      </c>
+      <c r="T9" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="U9" s="16">
+        <f t="shared" ref="U9:U10" si="18">((T9-1)*25) +(S9)</f>
+        <v>332</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" ref="W4:W10" si="19">CODE(LEFT(V9,1)) -64</f>
+        <v>23</v>
+      </c>
+      <c r="X9" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v>25</v>
+      </c>
+      <c r="Y9" s="16">
+        <f t="shared" ref="Y9:Y10" si="20">((X9-1)*25) +(W9)</f>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E10" s="19">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="H10" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="I10" s="19">
+        <f t="shared" si="14"/>
+        <v>269</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="L10" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="M10" s="19">
+        <f t="shared" si="15"/>
+        <v>443</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" s="17">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="P10" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="Q10" s="19">
+        <f t="shared" si="16"/>
+        <v>463</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="T10" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v>/////</v>
+      </c>
+      <c r="U10" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="W10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="X10" s="18" t="str">
+        <f t="shared" si="13"/>
+        <v>/////</v>
+      </c>
+      <c r="Y10" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="14">
+        <f>CODE(LEFT(B15,1)) -64</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="18" t="str">
+        <f>MID(B15,2,LEN(B15) -1)</f>
+        <v>14</v>
+      </c>
+      <c r="E15" s="19">
+        <f>((D15-1)*D19) +(C15)</f>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="14">
+        <f>CODE(LEFT(B23,1)) -64</f>
+        <v>2</v>
+      </c>
+      <c r="D23" s="18" t="str">
+        <f>MID(B23,2,LEN(B23) -1)</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="19">
+        <f>((D23-1)*25) +(C23)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3002,12 +4078,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Updated the Layout Map, a few errors on it
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
     <sheet name="Cell Calculator and Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Room Legend" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="83">
   <si>
     <t>X</t>
   </si>
@@ -269,17 +269,14 @@
     <t>///////</t>
   </si>
   <si>
-    <t>/////</t>
-  </si>
-  <si>
-    <t>A14</t>
+    <t>B13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,8 +341,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +423,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -468,15 +479,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -508,7 +510,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0">
@@ -589,8 +591,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyBorder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -617,21 +677,21 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="75" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="75" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="75" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="75" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="75" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="75" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="75" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="75" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="75" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="75" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="134">
     <cellStyle name="Closet" xfId="1"/>
     <cellStyle name="Doors" xfId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -669,6 +729,35 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -704,6 +793,35 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Room" xfId="2"/>
     <cellStyle name="Style 1" xfId="75"/>
@@ -1006,44 +1124,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:AM37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="5" max="5" width="4.5" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="13" width="4.42578125" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.85546875" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" customWidth="1"/>
-    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.33203125" customWidth="1"/>
+    <col min="9" max="10" width="4.5" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" customWidth="1"/>
+    <col min="12" max="13" width="4.5" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.83203125" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5" customWidth="1"/>
+    <col min="21" max="21" width="5.5" customWidth="1"/>
+    <col min="22" max="22" width="5.1640625" customWidth="1"/>
+    <col min="23" max="23" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="5.7109375" customWidth="1"/>
-    <col min="26" max="29" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.6640625" customWidth="1"/>
+    <col min="26" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6" customWidth="1"/>
-    <col min="31" max="31" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.140625" customWidth="1"/>
-    <col min="33" max="38" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.1640625" customWidth="1"/>
+    <col min="33" max="38" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1123,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1203,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1283,7 +1401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1363,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1523,7 +1641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +1721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1683,7 +1801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1763,7 +1881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1843,7 +1961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1926,7 +2044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2009,7 +2127,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -2092,7 +2210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2175,7 +2293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2376,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2341,7 +2459,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2424,7 +2542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2507,7 +2625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2590,7 +2708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30">
       <c r="A20" s="9" t="s">
         <v>1</v>
       </c>
@@ -2673,7 +2791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -2756,7 +2874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2919,7 +3037,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -2999,7 +3117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3197,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3154,6 +3272,56 @@
       </c>
       <c r="Y26">
         <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3169,47 +3337,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="H2" s="26" t="s">
@@ -3218,10 +3386,10 @@
       <c r="I2" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="L2" s="26" t="s">
@@ -3230,10 +3398,10 @@
       <c r="M2" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="P2" s="26" t="s">
@@ -3242,10 +3410,10 @@
       <c r="Q2" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="T2" s="26" t="s">
@@ -3254,820 +3422,982 @@
       <c r="U2" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="X2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="14">
-        <f>CODE(LEFT(B3,1)) -64</f>
+      <c r="C3" s="15">
+        <f>CODE(LEFT(B3,1)) -65</f>
+        <v>16</v>
+      </c>
+      <c r="D3" s="15">
+        <f>MID(B3,2,LEN(B3) -1) - 1</f>
+        <v>12</v>
+      </c>
+      <c r="E3" s="15">
+        <f>((D3)*25) +(C3) +1</f>
+        <v>317</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="15">
+        <f>CODE(LEFT(F3,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="H3" s="15">
+        <f>MID(F3,2,LEN(F3) -1) - 1</f>
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="str">
-        <f>MID(B3,2,LEN(B3) -1)</f>
-        <v>13</v>
-      </c>
-      <c r="E3" s="16">
-        <f>((D3-1)*25) +(C3)</f>
-        <v>317</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="14">
-        <f>CODE(LEFT(F3,1)) -64</f>
+      <c r="I3" s="15">
+        <f>((H3)*25) +(G3) +1</f>
+        <v>435</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="15" t="str">
+        <f t="shared" ref="L3" si="0">MID(J3,2,LEN(J3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="15" t="str">
+        <f t="shared" ref="P3" si="1">MID(N3,2,LEN(N3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="15" t="str">
+        <f t="shared" ref="T3:T11" si="2">MID(R3,2,LEN(R3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X3" s="15" t="str">
+        <f t="shared" ref="X3" si="3">MID(V3,2,LEN(V3) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="B4" s="19"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="15">
+        <f>CODE(LEFT(B5,1)) -65</f>
+        <v>16</v>
+      </c>
+      <c r="D5" s="15">
+        <f>MID(B5,2,LEN(B5) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="E5" s="15">
+        <f>((D5)*25) +(C5) +1</f>
+        <v>617</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="15">
+        <f>CODE(LEFT(F5,1)) -65</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <f>MID(F5,2,LEN(F5) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="I5" s="15">
+        <f>((H5)*25) +(G5) +1</f>
+        <v>476</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="15">
+        <f>CODE(LEFT(J5,1)) -65</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="15">
+        <f>MID(J5,2,LEN(J5) -1) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <f>((L5)*25) +(K5) +1</f>
+        <v>6</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="15">
+        <f>CODE(LEFT(N5,1)) -65</f>
+        <v>24</v>
+      </c>
+      <c r="P5" s="15">
+        <f>MID(N5,2,LEN(N5) -1) - 1</f>
+        <v>14</v>
+      </c>
+      <c r="Q5" s="15">
+        <f>((P5)*25) +(O5) +1</f>
+        <v>375</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v>/////</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X5" s="15" t="str">
+        <f t="shared" ref="X5" si="4">MID(V5,2,LEN(V5) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="15">
+        <f>CODE(LEFT(B7,1)) -65</f>
+        <v>7</v>
+      </c>
+      <c r="D7" s="15">
+        <f>MID(B7,2,LEN(B7) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="E7" s="15">
+        <f>((D7)*25) +(C7) +1</f>
+        <v>608</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="15">
+        <f>CODE(LEFT(F7,1)) -65</f>
+        <v>11</v>
+      </c>
+      <c r="H7" s="15">
+        <f>MID(F7,2,LEN(F7) -1) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="I7" s="15">
+        <f>((H7)*25) +(G7) +1</f>
+        <v>112</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" s="15" t="str">
+        <f t="shared" ref="L7" si="5">MID(J7,2,LEN(J7) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="15" t="str">
+        <f t="shared" ref="P7" si="6">MID(N7,2,LEN(N7) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T7" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v>/////</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" s="15" t="str">
+        <f t="shared" ref="X7" si="7">MID(V7,2,LEN(V7) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="15">
+        <f>CODE(LEFT(B9,1)) -65</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="15">
+        <f>MID(B9,2,LEN(B9) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="15">
+        <f>((D9)*25) +(C9) +1</f>
+        <v>80</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="15">
+        <f>CODE(LEFT(F9,1)) -65</f>
+        <v>18</v>
+      </c>
+      <c r="H9" s="15">
+        <f>MID(F9,2,LEN(F9) -1) - 1</f>
         <v>10</v>
       </c>
-      <c r="H3" s="15" t="str">
-        <f>MID(F3,2,LEN(F3) -1)</f>
+      <c r="I9" s="15">
+        <f>((H9)*25) +(G9) +1</f>
+        <v>269</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="15">
+        <f>CODE(LEFT(J9,1)) -65</f>
+        <v>17</v>
+      </c>
+      <c r="L9" s="15">
+        <f>MID(J9,2,LEN(J9) -1) - 1</f>
+        <v>17</v>
+      </c>
+      <c r="M9" s="15">
+        <f>((L9)*25) +(K9) +1</f>
+        <v>443</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="15">
+        <f>CODE(LEFT(N9,1)) -65</f>
+        <v>12</v>
+      </c>
+      <c r="P9" s="15">
+        <f>MID(N9,2,LEN(N9) -1) - 1</f>
         <v>18</v>
       </c>
-      <c r="I3" s="16">
-        <f>((H3-1)*25) +(G3)</f>
-        <v>435</v>
-      </c>
-      <c r="J3" s="22" t="s">
+      <c r="Q9" s="15">
+        <f>((P9)*25) +(O9) +1</f>
+        <v>463</v>
+      </c>
+      <c r="R9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="15" t="str">
-        <f>MID(J3,2,LEN(J3) -1)</f>
+      <c r="S9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T9" s="15" t="str">
+        <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="M3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="22" t="s">
+      <c r="U9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P3" s="15" t="str">
-        <f>MID(N3,2,LEN(N3) -1)</f>
+      <c r="W9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X9" s="15" t="str">
+        <f t="shared" ref="X9" si="8">MID(V9,2,LEN(V9) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="R3" s="22" t="s">
+      <c r="Y9" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="15">
+        <f>CODE(LEFT(B11,1)) -65</f>
+        <v>12</v>
+      </c>
+      <c r="D11" s="15">
+        <f>MID(B11,2,LEN(B11) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="E11" s="15">
+        <f>((D11)*25) +(C11) +1</f>
+        <v>488</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="15">
+        <f>CODE(LEFT(F11,1)) -65</f>
+        <v>7</v>
+      </c>
+      <c r="H11" s="15">
+        <f>MID(F11,2,LEN(F11) -1) - 1</f>
+        <v>6</v>
+      </c>
+      <c r="I11" s="15">
+        <f>((H11)*25) +(G11) +1</f>
+        <v>158</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="15">
+        <f>CODE(LEFT(J11,1)) -65</f>
+        <v>18</v>
+      </c>
+      <c r="L11" s="15">
+        <f>MID(J11,2,LEN(J11) -1) - 1</f>
+        <v>16</v>
+      </c>
+      <c r="M11" s="15">
+        <f>((L11)*25) +(K11) +1</f>
+        <v>419</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T3" s="15" t="str">
-        <f>MID(R3,2,LEN(R3) -1)</f>
+      <c r="O11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" s="15" t="str">
+        <f t="shared" ref="P11:P13" si="9">MID(N11,2,LEN(N11) -1)</f>
         <v>/////</v>
       </c>
-      <c r="U3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="V3" s="22" t="s">
+      <c r="Q11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="W3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X3" s="15" t="str">
-        <f>MID(V3,2,LEN(V3) -1)</f>
+      <c r="S11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T11" s="15" t="str">
+        <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="Y3" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="14">
-        <f t="shared" ref="C4:C10" si="0">CODE(LEFT(B4,1)) -64</f>
-        <v>17</v>
-      </c>
-      <c r="D4" s="15" t="str">
-        <f>MID(B4,2,LEN(B4) -1)</f>
-        <v>25</v>
-      </c>
-      <c r="E4" s="16">
-        <f t="shared" ref="E4:E10" si="1">((D4-1)*25) +(C4)</f>
-        <v>617</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="14">
-        <f t="shared" ref="G4:G10" si="2">CODE(LEFT(F4,1)) -64</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="15" t="str">
-        <f>MID(F4,2,LEN(F4) -1)</f>
-        <v>20</v>
-      </c>
-      <c r="I4" s="16">
-        <f t="shared" ref="I4:I7" si="3">((H4-1)*25) +(G4)</f>
-        <v>476</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="14">
-        <f t="shared" ref="K4:K10" si="4">CODE(LEFT(J4,1)) -64</f>
-        <v>6</v>
-      </c>
-      <c r="L4" s="15" t="str">
-        <f>MID(J4,2,LEN(J4) -1)</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="16">
-        <f t="shared" ref="M4:M7" si="5">((L4-1)*25) +(K4)</f>
-        <v>6</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="14">
-        <f t="shared" ref="O4:O10" si="6">CODE(LEFT(N4,1)) -64</f>
-        <v>25</v>
-      </c>
-      <c r="P4" s="15" t="str">
-        <f>MID(N4,2,LEN(N4) -1)</f>
-        <v>15</v>
-      </c>
-      <c r="Q4" s="16">
-        <f t="shared" ref="Q4:Q6" si="7">((P4-1)*25) +(O4)</f>
-        <v>375</v>
-      </c>
-      <c r="R4" s="22" t="s">
+      <c r="U11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="S4" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T4" s="15" t="str">
-        <f>MID(R4,2,LEN(R4) -1)</f>
+      <c r="W11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X11" s="15" t="str">
+        <f t="shared" ref="X11" si="10">MID(V11,2,LEN(V11) -1)</f>
         <v>/////</v>
       </c>
-      <c r="U4" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="V4" s="22" t="s">
+      <c r="Y11" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="B12" s="19"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="W4" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X4" s="15" t="str">
-        <f>MID(V4,2,LEN(V4) -1)</f>
+      <c r="C13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="15" t="str">
+        <f t="shared" ref="D13" si="11">MID(B13,2,LEN(B13) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Y4" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="14">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D5" s="15" t="str">
-        <f t="shared" ref="D5:D10" si="8">MID(B5,2,LEN(B5) -1)</f>
-        <v>25</v>
-      </c>
-      <c r="E5" s="16">
-        <f t="shared" si="1"/>
-        <v>608</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="14">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="H5" s="15" t="str">
-        <f t="shared" ref="H5:H10" si="9">MID(F5,2,LEN(F5) -1)</f>
-        <v>5</v>
-      </c>
-      <c r="I5" s="16">
-        <f t="shared" si="3"/>
-        <v>112</v>
-      </c>
-      <c r="J5" s="22" t="s">
+      <c r="E13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="L5" s="15" t="str">
-        <f t="shared" ref="L5:L10" si="10">MID(J5,2,LEN(J5) -1)</f>
+      <c r="G13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="15" t="str">
+        <f t="shared" ref="H13" si="12">MID(F13,2,LEN(F13) -1)</f>
         <v>/////</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="N5" s="22" t="s">
+      <c r="I13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="O5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P5" s="15" t="str">
-        <f t="shared" ref="P5:P10" si="11">MID(N5,2,LEN(N5) -1)</f>
+      <c r="K13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="15" t="str">
+        <f t="shared" ref="L13" si="13">MID(J13,2,LEN(J13) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Q5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="R5" s="22" t="s">
+      <c r="M13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="S5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T5" s="15" t="str">
-        <f t="shared" ref="T5:U10" si="12">MID(R5,2,LEN(R5) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X5" s="15" t="str">
-        <f t="shared" ref="X5:X10" si="13">MID(V5,2,LEN(V5) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D6" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="E6" s="16">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="14">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="H6" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="I6" s="16">
-        <f t="shared" si="3"/>
-        <v>269</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="14">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="L6" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-      <c r="M6" s="16">
-        <f t="shared" si="5"/>
-        <v>443</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="14">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="P6" s="15" t="str">
-        <f t="shared" si="11"/>
-        <v>19</v>
-      </c>
-      <c r="Q6" s="16">
-        <f t="shared" si="7"/>
-        <v>463</v>
-      </c>
-      <c r="R6" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T6" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v>/////</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="V6" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="W6" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X6" s="15" t="str">
-        <f t="shared" si="13"/>
-        <v>/////</v>
-      </c>
-      <c r="Y6" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D7" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="E7" s="16">
-        <f t="shared" si="1"/>
-        <v>488</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="14">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="H7" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="I7" s="16">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="14">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="L7" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v>17</v>
-      </c>
-      <c r="M7" s="16">
-        <f t="shared" si="5"/>
-        <v>419</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P7" s="15" t="str">
-        <f t="shared" si="11"/>
-        <v>/////</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T7" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v>/////</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="V7" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="W7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X7" s="15" t="str">
-        <f t="shared" si="13"/>
-        <v>/////</v>
-      </c>
-      <c r="Y7" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>/////</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="O13" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15" t="str">
+      <c r="P13" s="15" t="str">
         <f t="shared" si="9"/>
         <v>/////</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="Q13" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="R13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="S13" s="15"/>
+      <c r="T13" s="15" t="str">
+        <f t="shared" ref="T13" si="14">MID(R13,2,LEN(R13) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X13" s="15" t="str">
+        <f t="shared" ref="X13:X16" si="15">MID(V13,2,LEN(V13) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="15">
+        <f>CODE(LEFT(B14,1)) -65</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="15">
+        <f>MID(B14,2,LEN(B14) -1) - 1</f>
+        <v>13</v>
+      </c>
+      <c r="E14" s="15">
+        <f>((D14)*25) +(C14) +1</f>
+        <v>328</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="15">
+        <f>CODE(LEFT(F14,1)) -65</f>
+        <v>11</v>
+      </c>
+      <c r="H14" s="15">
+        <f>MID(F14,2,LEN(F14) -1) - 1</f>
+        <v>8</v>
+      </c>
+      <c r="I14" s="15">
+        <f>((H14)*25) +(G14) +1</f>
+        <v>212</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="15">
+        <f>CODE(LEFT(J14,1)) -65</f>
+        <v>17</v>
+      </c>
+      <c r="L14" s="15">
+        <f>MID(J14,2,LEN(J14) -1) - 1</f>
+        <v>23</v>
+      </c>
+      <c r="M14" s="15">
+        <f>((L14)*25) +(K14) +1</f>
+        <v>593</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" s="15">
+        <f>CODE(LEFT(N14,1)) -65</f>
+        <v>10</v>
+      </c>
+      <c r="P14" s="15">
+        <f>MID(N14,2,LEN(N14) -1) - 1</f>
+        <v>8</v>
+      </c>
+      <c r="Q14" s="15">
+        <f>((P14)*25) +(O14) +1</f>
+        <v>211</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="S14" s="15">
+        <f>CODE(LEFT(R14,1)) -65</f>
+        <v>6</v>
+      </c>
+      <c r="T14" s="15">
+        <f>MID(R14,2,LEN(R14) -1) - 1</f>
+        <v>13</v>
+      </c>
+      <c r="U14" s="15">
+        <f>((T14)*25) +(S14) +1</f>
+        <v>332</v>
+      </c>
+      <c r="V14" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="W14" s="15">
+        <f>CODE(LEFT(V14,1)) -65</f>
+        <v>22</v>
+      </c>
+      <c r="X14" s="15">
+        <f>MID(V14,2,LEN(V14) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="Y14" s="15">
+        <f>((X14)*25) +(W14) +1</f>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="15">
+        <f>CODE(LEFT(B16,1)) -65</f>
+        <v>4</v>
+      </c>
+      <c r="D16" s="15">
+        <f>MID(B16,2,LEN(B16) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="E16" s="15">
+        <f>((D16)*25) +(C16) +1</f>
+        <v>80</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="15">
+        <f>CODE(LEFT(F16,1)) -65</f>
+        <v>18</v>
+      </c>
+      <c r="H16" s="15">
+        <f>MID(F16,2,LEN(F16) -1) - 1</f>
+        <v>10</v>
+      </c>
+      <c r="I16" s="15">
+        <f>((H16)*25) +(G16) +1</f>
+        <v>269</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="15">
+        <f>CODE(LEFT(J16,1)) -65</f>
+        <v>17</v>
+      </c>
+      <c r="L16" s="15">
+        <f>MID(J16,2,LEN(J16) -1) - 1</f>
+        <v>17</v>
+      </c>
+      <c r="M16" s="15">
+        <f>((L16)*25) +(K16) +1</f>
+        <v>443</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="15">
+        <f>CODE(LEFT(N16,1)) -65</f>
+        <v>12</v>
+      </c>
+      <c r="P16" s="15">
+        <f>MID(N16,2,LEN(N16) -1) - 1</f>
+        <v>18</v>
+      </c>
+      <c r="Q16" s="15">
+        <f>((P16)*25) +(O16) +1</f>
+        <v>463</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="T16" s="15" t="str">
+        <f t="shared" ref="T16" si="16">MID(R16,2,LEN(R16) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="V16" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="W16" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X16" s="15" t="str">
+        <f t="shared" ref="X16" si="17">MID(V16,2,LEN(V16) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y16" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v>/////</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="N8" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P8" s="15" t="str">
-        <f t="shared" si="11"/>
-        <v>/////</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="T8" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v>/////</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="V8" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="W8" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="X8" s="15" t="str">
-        <f t="shared" si="13"/>
-        <v>/////</v>
-      </c>
-      <c r="Y8" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="14">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D9" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-      <c r="E9" s="16">
-        <f t="shared" si="1"/>
-        <v>328</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="14">
-        <f t="shared" si="2"/>
+      <c r="C21" s="14">
+        <f>CODE(LEFT(B21,1)) -65</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="16">
+        <f>MID(B21,2,LEN(B21) -1) - 1</f>
         <v>12</v>
       </c>
-      <c r="H9" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="I9" s="16">
-        <f t="shared" ref="I9:I10" si="14">((H9-1)*25) +(G9)</f>
-        <v>212</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="K9" s="14">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="L9" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="M9" s="16">
-        <f t="shared" ref="M9:M10" si="15">((L9-1)*25) +(K9)</f>
-        <v>593</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="O9" s="14">
-        <f t="shared" si="6"/>
-        <v>11</v>
-      </c>
-      <c r="P9" s="15" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">9 </v>
-      </c>
-      <c r="Q9" s="16">
-        <f t="shared" ref="Q9:Q10" si="16">((P9-1)*25) +(O9)</f>
-        <v>211</v>
-      </c>
-      <c r="R9" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="S9" s="14">
-        <f t="shared" ref="S9" si="17">CODE(LEFT(R9,1)) -64</f>
-        <v>7</v>
-      </c>
-      <c r="T9" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v>14</v>
-      </c>
-      <c r="U9" s="16">
-        <f t="shared" ref="U9:U10" si="18">((T9-1)*25) +(S9)</f>
-        <v>332</v>
-      </c>
-      <c r="V9" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="W9" s="14">
-        <f t="shared" ref="W9" si="19">CODE(LEFT(V9,1)) -64</f>
-        <v>23</v>
-      </c>
-      <c r="X9" s="15" t="str">
-        <f t="shared" si="13"/>
+      <c r="E21" s="17">
+        <f>((D21)*D25) +(C21) + 1</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24">
         <v>25</v>
       </c>
-      <c r="Y9" s="16">
-        <f t="shared" ref="Y9" si="20">((X9-1)*25) +(W9)</f>
-        <v>623</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D10" s="18" t="str">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="E10" s="19">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="17">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="H10" s="18" t="str">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="I10" s="19">
-        <f t="shared" si="14"/>
-        <v>269</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="17">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="L10" s="18" t="str">
-        <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-      <c r="M10" s="19">
-        <f t="shared" si="15"/>
-        <v>443</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="17">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="P10" s="18" t="str">
-        <f t="shared" si="11"/>
-        <v>19</v>
-      </c>
-      <c r="Q10" s="19">
-        <f t="shared" si="16"/>
-        <v>463</v>
-      </c>
-      <c r="R10" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="S10" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="T10" s="18" t="str">
-        <f t="shared" si="12"/>
-        <v>/////</v>
-      </c>
-      <c r="U10" s="18" t="str">
-        <f t="shared" si="12"/>
-        <v>////</v>
-      </c>
-      <c r="V10" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="W10" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="X10" s="18" t="str">
-        <f t="shared" si="13"/>
-        <v>/////</v>
-      </c>
-      <c r="Y10" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="D25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D28" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E28" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="14">
-        <f>CODE(LEFT(B15,1)) -64</f>
-        <v>1</v>
-      </c>
-      <c r="D15" s="18" t="str">
-        <f>MID(B15,2,LEN(B15) -1)</f>
-        <v>14</v>
-      </c>
-      <c r="E15" s="19">
-        <f>((D15-1)*D19) +(C15)</f>
-        <v>326</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+    <row r="29" spans="2:5">
+      <c r="B29" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="14">
-        <f>CODE(LEFT(B23,1)) -64</f>
-        <v>2</v>
-      </c>
-      <c r="D23" s="18" t="str">
-        <f>MID(B23,2,LEN(B23) -1)</f>
-        <v>1</v>
-      </c>
-      <c r="E23" s="19">
-        <f>((D23-1)*25) +(C23)</f>
+      <c r="C29" s="14">
+        <f>CODE(LEFT(B29,1)) -65</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="16">
+        <f>MID(B29,2,LEN(B29) -1) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="17">
+        <f>((D29)*D33) +(C29) + 1</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="H13 D13 L13 L7 P9 T14 X14 P5 L5 P7" formula="1"/>
+    <ignoredError sqref="E29" emptyCellReference="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4084,64 +4414,64 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Updated Layout Again to match the tests, haven't pushed test changes, will come in next commit
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="84">
   <si>
     <t>X</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>B13</t>
+  </si>
+  <si>
+    <t>P5</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="134">
+  <cellStyleXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0">
@@ -591,6 +594,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyBorder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -691,7 +698,7 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="75" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="134">
+  <cellStyles count="138">
     <cellStyle name="Closet" xfId="1"/>
     <cellStyle name="Doors" xfId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -758,6 +765,8 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -822,6 +831,8 @@
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Room" xfId="2"/>
     <cellStyle name="Style 1" xfId="75"/>
@@ -1127,7 +1138,7 @@
   <dimension ref="A1:AD39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1527,7 +1538,7 @@
       <c r="O5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -2016,7 +2027,7 @@
       <c r="R11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="S11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="4" t="s">
@@ -3339,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3798,19 +3809,19 @@
         <v>80</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G9" s="15">
         <f>CODE(LEFT(F9,1)) -65</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" s="15">
         <f>MID(F9,2,LEN(F9) -1) - 1</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I9" s="15">
         <f>((H9)*25) +(G9) +1</f>
-        <v>269</v>
+        <v>116</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
UPDATED ALL ADJACENCY TESTS WITH LAYOUT MAP, Also, updated Layout Map; started working on some logic with adjacency tests, but tests are all set up (fail right now)
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560"/>
+    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="93">
   <si>
     <t>X</t>
   </si>
@@ -206,9 +206,6 @@
     <t>M20</t>
   </si>
   <si>
-    <t>H7</t>
-  </si>
-  <si>
     <t>S17</t>
   </si>
   <si>
@@ -273,6 +270,36 @@
   </si>
   <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Tan Pink: Locations inside rooms, adjacency test</t>
+  </si>
+  <si>
+    <t>Tan Pink: Locations inside a room, adjacency tests</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>V20</t>
   </si>
 </sst>
 </file>
@@ -353,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF800000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,7 +546,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0">
@@ -656,8 +689,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -697,8 +742,11 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="75" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="150">
     <cellStyle name="Closet" xfId="1"/>
     <cellStyle name="Doors" xfId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -767,6 +815,12 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -833,6 +887,12 @@
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Room" xfId="2"/>
     <cellStyle name="Style 1" xfId="75"/>
@@ -1135,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD39"/>
+  <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1173,7 +1233,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1422,7 +1482,7 @@
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="13" t="s">
@@ -1458,7 +1518,7 @@
       <c r="O4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="Q4" s="4" t="s">
@@ -1473,7 +1533,7 @@
       <c r="T4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="27" t="s">
         <v>10</v>
       </c>
       <c r="V4" s="2" t="s">
@@ -1674,13 +1734,13 @@
       <c r="G7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -1862,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>1</v>
@@ -2145,7 +2205,7 @@
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2747,7 +2807,7 @@
       <c r="I20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="27" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
@@ -2783,7 +2843,7 @@
       <c r="U20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V20" s="4" t="s">
+      <c r="V20" s="27" t="s">
         <v>4</v>
       </c>
       <c r="W20" s="4" t="s">
@@ -3321,17 +3381,22 @@
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="12" t="s">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="12" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3348,10 +3413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3366,7 +3431,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3374,76 +3439,76 @@
         <v>38</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="D2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="L2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="P2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="25" t="s">
+      <c r="S2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="T2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="V2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="V2" s="25" t="s">
+      <c r="W2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="26" t="s">
-        <v>72</v>
-      </c>
       <c r="X2" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y2" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -3481,56 +3546,56 @@
         <v>435</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" s="15" t="str">
         <f t="shared" ref="L3" si="0">MID(J3,2,LEN(J3) -1)</f>
         <v>/////</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P3" s="15" t="str">
         <f t="shared" ref="P3" si="1">MID(N3,2,LEN(N3) -1)</f>
         <v>/////</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T3" s="15" t="str">
         <f t="shared" ref="T3:T11" si="2">MID(R3,2,LEN(R3) -1)</f>
         <v>/////</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X3" s="15" t="str">
         <f t="shared" ref="X3" si="3">MID(V3,2,LEN(V3) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -3624,30 +3689,30 @@
         <v>375</v>
       </c>
       <c r="R5" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T5" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X5" s="15" t="str">
         <f t="shared" ref="X5" si="4">MID(V5,2,LEN(V5) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -3711,56 +3776,56 @@
         <v>112</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L7" s="15" t="str">
         <f t="shared" ref="L7" si="5">MID(J7,2,LEN(J7) -1)</f>
         <v>/////</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P7" s="15" t="str">
         <f t="shared" ref="P7" si="6">MID(N7,2,LEN(N7) -1)</f>
         <v>/////</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T7" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
       <c r="U7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V7" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X7" s="15" t="str">
         <f t="shared" ref="X7" si="7">MID(V7,2,LEN(V7) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -3809,7 +3874,7 @@
         <v>80</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="15">
         <f>CODE(LEFT(F9,1)) -65</f>
@@ -3854,30 +3919,30 @@
         <v>463</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T9" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V9" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X9" s="15" t="str">
         <f t="shared" ref="X9" si="8">MID(V9,2,LEN(V9) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -3926,22 +3991,22 @@
         <v>488</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="G11" s="15">
         <f>CODE(LEFT(F11,1)) -65</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H11" s="15">
         <f>MID(F11,2,LEN(F11) -1) - 1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I11" s="15">
         <f>((H11)*25) +(G11) +1</f>
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11" s="15">
         <f>CODE(LEFT(J11,1)) -65</f>
@@ -3956,43 +4021,45 @@
         <v>419</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="P11" s="15" t="str">
-        <f t="shared" ref="P11:P13" si="9">MID(N11,2,LEN(N11) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Q11" s="15" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="O11" s="15">
+        <f>CODE(LEFT(N11,1)) -65</f>
+        <v>3</v>
+      </c>
+      <c r="P11" s="15">
+        <f>MID(N11,2,LEN(N11) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="Q11" s="15">
+        <f>((P11)*25) +(O11) +1</f>
+        <v>79</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T11" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
       <c r="U11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V11" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X11" s="15" t="str">
-        <f t="shared" ref="X11" si="10">MID(V11,2,LEN(V11) -1)</f>
+        <f t="shared" ref="X11" si="9">MID(V11,2,LEN(V11) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -4022,243 +4089,243 @@
       <c r="Y12" s="15"/>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="15">
+        <f>CODE(LEFT(B13,1)) -65</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <f>MID(B13,2,LEN(B13) -1) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <f>((D13)*25) +(C13) +1</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="15">
+        <f>CODE(LEFT(F13,1)) -65</f>
+        <v>2</v>
+      </c>
+      <c r="H13" s="15">
+        <f>MID(F13,2,LEN(F13) -1) - 1</f>
+        <v>12</v>
+      </c>
+      <c r="I13" s="15">
+        <f>((H13)*25) +(G13) +1</f>
+        <v>303</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="15">
+        <f>CODE(LEFT(J13,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="L13" s="15">
+        <f>MID(J13,2,LEN(J13) -1) - 1</f>
+        <v>6</v>
+      </c>
+      <c r="M13" s="15">
+        <f>((L13)*25) +(K13) +1</f>
+        <v>160</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="O13" s="15">
+        <f>CODE(LEFT(N13,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="P13" s="15">
+        <f>MID(N13,2,LEN(N13) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="Q13" s="15">
+        <f>((P13)*25) +(O13) +1</f>
+        <v>485</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="S13" s="15">
+        <f>CODE(LEFT(R13,1)) -65</f>
+        <v>20</v>
+      </c>
+      <c r="T13" s="15">
+        <f>MID(R13,2,LEN(R13) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="U13" s="15">
+        <f>((T13)*25) +(S13) +1</f>
+        <v>96</v>
+      </c>
+      <c r="V13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="W13" s="15">
+        <f>CODE(LEFT(V13,1)) -65</f>
+        <v>21</v>
+      </c>
+      <c r="X13" s="15">
+        <f>MID(V13,2,LEN(V13) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="Y13" s="15">
+        <f>((X13)*25) +(W13) +1</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="15" t="str">
-        <f t="shared" ref="D13" si="11">MID(B13,2,LEN(B13) -1)</f>
+      <c r="B15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="15" t="str">
+        <f t="shared" ref="D15" si="10">MID(B15,2,LEN(B15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="15" t="str">
-        <f t="shared" ref="H13" si="12">MID(F13,2,LEN(F13) -1)</f>
+      <c r="E15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="15" t="str">
+        <f t="shared" ref="H15" si="11">MID(F15,2,LEN(F15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="I13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="15" t="str">
-        <f t="shared" ref="L13" si="13">MID(J13,2,LEN(J13) -1)</f>
+      <c r="I15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="15" t="str">
+        <f t="shared" ref="L15" si="12">MID(J15,2,LEN(J15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="M13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="P13" s="15" t="str">
-        <f t="shared" si="9"/>
+      <c r="M15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="P15" s="15" t="str">
+        <f t="shared" ref="P11:P15" si="13">MID(N15,2,LEN(N15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Q13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="R13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15" t="str">
-        <f t="shared" ref="T13" si="14">MID(R13,2,LEN(R13) -1)</f>
+      <c r="Q15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15" t="str">
+        <f t="shared" ref="T15" si="14">MID(R15,2,LEN(R15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="U13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="V13" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="W13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="X13" s="15" t="str">
-        <f t="shared" ref="X13:X16" si="15">MID(V13,2,LEN(V13) -1)</f>
+      <c r="U15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="V15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="X15" s="15" t="str">
+        <f t="shared" ref="X15:X18" si="15">MID(V15,2,LEN(V15) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Y13" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="15">
-        <f>CODE(LEFT(B14,1)) -65</f>
-        <v>2</v>
-      </c>
-      <c r="D14" s="15">
-        <f>MID(B14,2,LEN(B14) -1) - 1</f>
-        <v>13</v>
-      </c>
-      <c r="E14" s="15">
-        <f>((D14)*25) +(C14) +1</f>
-        <v>328</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="15">
-        <f>CODE(LEFT(F14,1)) -65</f>
-        <v>11</v>
-      </c>
-      <c r="H14" s="15">
-        <f>MID(F14,2,LEN(F14) -1) - 1</f>
-        <v>8</v>
-      </c>
-      <c r="I14" s="15">
-        <f>((H14)*25) +(G14) +1</f>
-        <v>212</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" s="15">
-        <f>CODE(LEFT(J14,1)) -65</f>
-        <v>17</v>
-      </c>
-      <c r="L14" s="15">
-        <f>MID(J14,2,LEN(J14) -1) - 1</f>
-        <v>23</v>
-      </c>
-      <c r="M14" s="15">
-        <f>((L14)*25) +(K14) +1</f>
-        <v>593</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="O14" s="15">
-        <f>CODE(LEFT(N14,1)) -65</f>
-        <v>10</v>
-      </c>
-      <c r="P14" s="15">
-        <f>MID(N14,2,LEN(N14) -1) - 1</f>
-        <v>8</v>
-      </c>
-      <c r="Q14" s="15">
-        <f>((P14)*25) +(O14) +1</f>
-        <v>211</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="S14" s="15">
-        <f>CODE(LEFT(R14,1)) -65</f>
-        <v>6</v>
-      </c>
-      <c r="T14" s="15">
-        <f>MID(R14,2,LEN(R14) -1) - 1</f>
-        <v>13</v>
-      </c>
-      <c r="U14" s="15">
-        <f>((T14)*25) +(S14) +1</f>
-        <v>332</v>
-      </c>
-      <c r="V14" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="W14" s="15">
-        <f>CODE(LEFT(V14,1)) -65</f>
-        <v>22</v>
-      </c>
-      <c r="X14" s="15">
-        <f>MID(V14,2,LEN(V14) -1) - 1</f>
-        <v>24</v>
-      </c>
-      <c r="Y14" s="15">
-        <f>((X14)*25) +(W14) +1</f>
-        <v>623</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
+      <c r="Y15" s="15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C16" s="15">
         <f>CODE(LEFT(B16,1)) -65</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" s="15">
         <f>MID(B16,2,LEN(B16) -1) - 1</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E16" s="15">
         <f>((D16)*25) +(C16) +1</f>
-        <v>80</v>
+        <v>328</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G16" s="15">
         <f>CODE(LEFT(F16,1)) -65</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H16" s="15">
         <f>MID(F16,2,LEN(F16) -1) - 1</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I16" s="15">
         <f>((H16)*25) +(G16) +1</f>
-        <v>269</v>
+        <v>212</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="K16" s="15">
         <f>CODE(LEFT(J16,1)) -65</f>
@@ -4266,139 +4333,260 @@
       </c>
       <c r="L16" s="15">
         <f>MID(J16,2,LEN(J16) -1) - 1</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="M16" s="15">
         <f>((L16)*25) +(K16) +1</f>
-        <v>443</v>
+        <v>593</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="O16" s="15">
         <f>CODE(LEFT(N16,1)) -65</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P16" s="15">
         <f>MID(N16,2,LEN(N16) -1) - 1</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="15">
         <f>((P16)*25) +(O16) +1</f>
+        <v>211</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" s="15">
+        <f>CODE(LEFT(R16,1)) -65</f>
+        <v>6</v>
+      </c>
+      <c r="T16" s="15">
+        <f>MID(R16,2,LEN(R16) -1) - 1</f>
+        <v>13</v>
+      </c>
+      <c r="U16" s="15">
+        <f>((T16)*25) +(S16) +1</f>
+        <v>332</v>
+      </c>
+      <c r="V16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="W16" s="15">
+        <f>CODE(LEFT(V16,1)) -65</f>
+        <v>22</v>
+      </c>
+      <c r="X16" s="15">
+        <f>MID(V16,2,LEN(V16) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="Y16" s="15">
+        <f>((X16)*25) +(W16) +1</f>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="15">
+        <f>CODE(LEFT(B18,1)) -65</f>
+        <v>4</v>
+      </c>
+      <c r="D18" s="15">
+        <f>MID(B18,2,LEN(B18) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="15">
+        <f>((D18)*25) +(C18) +1</f>
+        <v>80</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="15">
+        <f>CODE(LEFT(F18,1)) -65</f>
+        <v>18</v>
+      </c>
+      <c r="H18" s="15">
+        <f>MID(F18,2,LEN(F18) -1) - 1</f>
+        <v>10</v>
+      </c>
+      <c r="I18" s="15">
+        <f>((H18)*25) +(G18) +1</f>
+        <v>269</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="15">
+        <f>CODE(LEFT(J18,1)) -65</f>
+        <v>17</v>
+      </c>
+      <c r="L18" s="15">
+        <f>MID(J18,2,LEN(J18) -1) - 1</f>
+        <v>17</v>
+      </c>
+      <c r="M18" s="15">
+        <f>((L18)*25) +(K18) +1</f>
+        <v>443</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="15">
+        <f>CODE(LEFT(N18,1)) -65</f>
+        <v>12</v>
+      </c>
+      <c r="P18" s="15">
+        <f>MID(N18,2,LEN(N18) -1) - 1</f>
+        <v>18</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>((P18)*25) +(O18) +1</f>
         <v>463</v>
       </c>
-      <c r="R16" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="S16" s="15" t="s">
+      <c r="R18" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="T18" s="15" t="str">
+        <f t="shared" ref="T18" si="16">MID(R18,2,LEN(R18) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="V18" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="X18" s="15" t="str">
+        <f t="shared" ref="X18" si="17">MID(V18,2,LEN(V18) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y18" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="B22" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="B23" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="T16" s="15" t="str">
-        <f t="shared" ref="T16" si="16">MID(R16,2,LEN(R16) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="U16" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="V16" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="W16" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="X16" s="15" t="str">
-        <f t="shared" ref="X16" si="17">MID(V16,2,LEN(V16) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y16" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+      <c r="C23" s="14">
+        <f>CODE(LEFT(B23,1)) -65</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="16">
+        <f>MID(B23,2,LEN(B23) -1) - 1</f>
+        <v>12</v>
+      </c>
+      <c r="E23" s="17">
+        <f>((D23)*D27) +(C23) + 1</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="B29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="20" t="s">
+    <row r="30" spans="1:25">
+      <c r="B30" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="14">
-        <f>CODE(LEFT(B21,1)) -65</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="16">
-        <f>MID(B21,2,LEN(B21) -1) - 1</f>
-        <v>12</v>
-      </c>
-      <c r="E21" s="17">
-        <f>((D21)*D25) +(C21) + 1</f>
-        <v>302</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
+      <c r="D30" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="B31" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="14">
-        <f>CODE(LEFT(B29,1)) -65</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="16">
-        <f>MID(B29,2,LEN(B29) -1) - 1</f>
+      <c r="C31" s="14">
+        <f>CODE(LEFT(B31,1)) -65</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="16">
+        <f>MID(B31,2,LEN(B31) -1) - 1</f>
         <v>0</v>
       </c>
-      <c r="E29" s="17">
-        <f>((D29)*D33) +(C29) + 1</f>
+      <c r="E31" s="17">
+        <f>((D31)*D35) +(C31) + 1</f>
         <v>2</v>
       </c>
     </row>
@@ -4406,8 +4594,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="H13 D13 L13 L7 P9 T14 X14 P5 L5 P7" formula="1"/>
-    <ignoredError sqref="E29" emptyCellReference="1"/>
+    <ignoredError sqref="H15 D15 L15 L7 P9 T16 X16 P5 L5 P7" formula="1"/>
+    <ignoredError sqref="E31" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
All adjacency tests now work; now working on target testing
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560" activeTab="1"/>
+    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
     <sheet name="Cell Calculator and Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Room Legend" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="92">
   <si>
     <t>X</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>///////</t>
-  </si>
-  <si>
-    <t>B13</t>
   </si>
   <si>
     <t>P5</t>
@@ -1197,42 +1194,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" customWidth="1"/>
-    <col min="5" max="5" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="8" width="4.33203125" customWidth="1"/>
-    <col min="9" max="10" width="4.5" customWidth="1"/>
-    <col min="11" max="11" width="4.1640625" customWidth="1"/>
-    <col min="12" max="13" width="4.5" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" customWidth="1"/>
-    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.83203125" customWidth="1"/>
-    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5" customWidth="1"/>
-    <col min="21" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="22" width="5.1640625" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.28515625" customWidth="1"/>
+    <col min="9" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+    <col min="12" max="13" width="4.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.85546875" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="5.6640625" customWidth="1"/>
-    <col min="26" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" customWidth="1"/>
+    <col min="26" max="29" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6" customWidth="1"/>
-    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.1640625" customWidth="1"/>
-    <col min="33" max="38" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" customWidth="1"/>
+    <col min="33" max="38" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1472,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1632,7 +1629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1712,7 +1709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1792,7 +1789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1872,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1952,7 +1949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2032,7 +2029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2115,7 +2112,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2198,7 +2195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -2281,7 +2278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2696,7 +2693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2779,7 +2776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>1</v>
       </c>
@@ -2862,7 +2859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -2945,7 +2942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -3028,7 +3025,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -3108,7 +3105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -3188,7 +3185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -3268,7 +3265,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3345,57 +3342,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -3415,18 +3412,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
@@ -3434,7 +3431,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -3511,7 +3508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3598,7 +3595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="19"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -3624,7 +3621,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3715,7 +3712,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="19"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -3741,7 +3738,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3828,7 +3825,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -3854,7 +3851,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -3874,7 +3871,7 @@
         <v>80</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="15">
         <f>CODE(LEFT(F9,1)) -65</f>
@@ -3945,7 +3942,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3971,7 +3968,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -3991,7 +3988,7 @@
         <v>488</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G11" s="15">
         <f>CODE(LEFT(F11,1)) -65</f>
@@ -4021,7 +4018,7 @@
         <v>419</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" s="15">
         <f>CODE(LEFT(N11,1)) -65</f>
@@ -4062,7 +4059,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -4088,12 +4085,12 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>87</v>
       </c>
       <c r="C13" s="15">
         <f>CODE(LEFT(B13,1)) -65</f>
@@ -4108,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="15">
         <f>CODE(LEFT(F13,1)) -65</f>
@@ -4123,7 +4120,7 @@
         <v>303</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K13" s="15">
         <f>CODE(LEFT(J13,1)) -65</f>
@@ -4138,7 +4135,7 @@
         <v>160</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O13" s="15">
         <f>CODE(LEFT(N13,1)) -65</f>
@@ -4153,7 +4150,7 @@
         <v>485</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S13" s="15">
         <f>CODE(LEFT(R13,1)) -65</f>
@@ -4168,7 +4165,7 @@
         <v>96</v>
       </c>
       <c r="V13" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W13" s="15">
         <f>CODE(LEFT(V13,1)) -65</f>
@@ -4183,7 +4180,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -4209,7 +4206,7 @@
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
@@ -4259,7 +4256,7 @@
         <v>80</v>
       </c>
       <c r="P15" s="15" t="str">
-        <f t="shared" ref="P11:P15" si="13">MID(N15,2,LEN(N15) -1)</f>
+        <f t="shared" ref="P15" si="13">MID(N15,2,LEN(N15) -1)</f>
         <v>/////</v>
       </c>
       <c r="Q15" s="15" t="s">
@@ -4283,14 +4280,14 @@
         <v>80</v>
       </c>
       <c r="X15" s="15" t="str">
-        <f t="shared" ref="X15:X18" si="15">MID(V15,2,LEN(V15) -1)</f>
+        <f t="shared" ref="X15" si="15">MID(V15,2,LEN(V15) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y15" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -4385,7 +4382,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -4411,7 +4408,7 @@
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4502,12 +4499,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>70</v>
       </c>
@@ -4521,13 +4518,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C23" s="14">
         <f>CODE(LEFT(B23,1)) -65</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="16">
         <f>MID(B23,2,LEN(B23) -1) - 1</f>
@@ -4535,10 +4532,10 @@
       </c>
       <c r="E23" s="17">
         <f>((D23)*D27) +(C23) + 1</f>
-        <v>302</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -4546,7 +4543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -4554,12 +4551,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>70</v>
       </c>
@@ -4573,7 +4570,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>77</v>
       </c>
@@ -4613,64 +4610,64 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Step target tests have correct numbers and updated layout
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15600"/>
+    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="93">
   <si>
     <t>X</t>
   </si>
@@ -224,9 +224,6 @@
     <t>L9</t>
   </si>
   <si>
-    <t>R24</t>
-  </si>
-  <si>
     <t>W25</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>//////</t>
   </si>
   <si>
-    <t>CELL CALCULATOR FOR TESTS</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -297,6 +291,15 @@
   </si>
   <si>
     <t>V20</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>V14</t>
+  </si>
+  <si>
+    <t>//////////</t>
   </si>
 </sst>
 </file>
@@ -699,7 +702,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
@@ -734,9 +737,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="75" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="75" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="75" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="75" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1230,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1530,7 +1530,7 @@
       <c r="T4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="26" t="s">
         <v>10</v>
       </c>
       <c r="V4" s="2" t="s">
@@ -1737,7 +1737,7 @@
       <c r="I7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -2202,7 +2202,7 @@
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2336,13 +2336,13 @@
       <c r="S14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="V14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="W14" s="2" t="s">
@@ -2804,7 +2804,7 @@
       <c r="I20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
@@ -2840,7 +2840,7 @@
       <c r="U20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V20" s="27" t="s">
+      <c r="V20" s="26" t="s">
         <v>4</v>
       </c>
       <c r="W20" s="4" t="s">
@@ -3157,7 +3157,7 @@
       <c r="Q24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R24" s="11" t="s">
+      <c r="R24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S24" s="2" t="s">
@@ -3379,7 +3379,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -3412,8 +3412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,875 +3429,957 @@
         <v>46</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="15">
+        <f>CODE(LEFT(B2,1)) -65</f>
+        <v>16</v>
+      </c>
+      <c r="D2" s="15">
+        <f>MID(B2,2,LEN(B2) -1) - 1</f>
+        <v>12</v>
+      </c>
+      <c r="E2" s="15">
+        <f>((D2)*25) +(C2) +1</f>
+        <v>317</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="15">
+        <f>CODE(LEFT(F2,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="H2" s="15">
+        <f>MID(F2,2,LEN(F2) -1) - 1</f>
+        <v>17</v>
+      </c>
+      <c r="I2" s="15">
+        <f>((H2)*25) +(G2) +1</f>
+        <v>435</v>
+      </c>
+      <c r="J2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="26" t="s">
+      <c r="K2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="15" t="str">
+        <f t="shared" ref="L2" si="0">MID(J2,2,LEN(J2) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="26" t="s">
+      <c r="O2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="15" t="str">
+        <f t="shared" ref="P2" si="1">MID(N2,2,LEN(N2) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="26" t="s">
+      <c r="S2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="15" t="str">
+        <f t="shared" ref="T2:T10" si="2">MID(R2,2,LEN(R2) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="26" t="s">
+      <c r="W2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="15" t="str">
+        <f t="shared" ref="X2" si="3">MID(V2,2,LEN(V2) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="15">
+        <f>CODE(LEFT(B4,1)) -65</f>
+        <v>16</v>
+      </c>
+      <c r="D4" s="15">
+        <f>MID(B4,2,LEN(B4) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="E4" s="15">
+        <f>((D4)*25) +(C4) +1</f>
+        <v>617</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="15">
+        <f>CODE(LEFT(F4,1)) -65</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="15">
+        <f>MID(F4,2,LEN(F4) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="I4" s="15">
+        <f>((H4)*25) +(G4) +1</f>
+        <v>476</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="15">
+        <f>CODE(LEFT(J4,1)) -65</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="15">
+        <f>MID(J4,2,LEN(J4) -1) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <f>((L4)*25) +(K4) +1</f>
+        <v>6</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="15">
+        <f>CODE(LEFT(N4,1)) -65</f>
+        <v>24</v>
+      </c>
+      <c r="P4" s="15">
+        <f>MID(N4,2,LEN(N4) -1) - 1</f>
+        <v>14</v>
+      </c>
+      <c r="Q4" s="15">
+        <f>((P4)*25) +(O4) +1</f>
+        <v>375</v>
+      </c>
+      <c r="R4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="V2" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="15">
-        <f>CODE(LEFT(B3,1)) -65</f>
-        <v>16</v>
-      </c>
-      <c r="D3" s="15">
-        <f>MID(B3,2,LEN(B3) -1) - 1</f>
-        <v>12</v>
-      </c>
-      <c r="E3" s="15">
-        <f>((D3)*25) +(C3) +1</f>
-        <v>317</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="15">
-        <f>CODE(LEFT(F3,1)) -65</f>
-        <v>9</v>
-      </c>
-      <c r="H3" s="15">
-        <f>MID(F3,2,LEN(F3) -1) - 1</f>
-        <v>17</v>
-      </c>
-      <c r="I3" s="15">
-        <f>((H3)*25) +(G3) +1</f>
-        <v>435</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" s="15" t="str">
-        <f t="shared" ref="L3" si="0">MID(J3,2,LEN(J3) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="P3" s="15" t="str">
-        <f t="shared" ref="P3" si="1">MID(N3,2,LEN(N3) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="T3" s="15" t="str">
-        <f t="shared" ref="T3:T11" si="2">MID(R3,2,LEN(R3) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X3" s="15" t="str">
-        <f t="shared" ref="X3" si="3">MID(V3,2,LEN(V3) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="15">
-        <f>CODE(LEFT(B5,1)) -65</f>
-        <v>16</v>
-      </c>
-      <c r="D5" s="15">
-        <f>MID(B5,2,LEN(B5) -1) - 1</f>
-        <v>24</v>
-      </c>
-      <c r="E5" s="15">
-        <f>((D5)*25) +(C5) +1</f>
-        <v>617</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="15">
-        <f>CODE(LEFT(F5,1)) -65</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="15">
-        <f>MID(F5,2,LEN(F5) -1) - 1</f>
-        <v>19</v>
-      </c>
-      <c r="I5" s="15">
-        <f>((H5)*25) +(G5) +1</f>
-        <v>476</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="15">
-        <f>CODE(LEFT(J5,1)) -65</f>
-        <v>5</v>
-      </c>
-      <c r="L5" s="15">
-        <f>MID(J5,2,LEN(J5) -1) - 1</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="15">
-        <f>((L5)*25) +(K5) +1</f>
-        <v>6</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="15">
-        <f>CODE(LEFT(N5,1)) -65</f>
-        <v>24</v>
-      </c>
-      <c r="P5" s="15">
-        <f>MID(N5,2,LEN(N5) -1) - 1</f>
-        <v>14</v>
-      </c>
-      <c r="Q5" s="15">
-        <f>((P5)*25) +(O5) +1</f>
-        <v>375</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="T5" s="15" t="str">
+      <c r="S4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="U5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X5" s="15" t="str">
-        <f t="shared" ref="X5" si="4">MID(V5,2,LEN(V5) -1)</f>
+      <c r="U4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X4" s="15" t="str">
+        <f t="shared" ref="X4" si="4">MID(V4,2,LEN(V4) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Y5" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="Y4" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="15">
-        <f>CODE(LEFT(B7,1)) -65</f>
-        <v>7</v>
-      </c>
-      <c r="D7" s="15">
-        <f>MID(B7,2,LEN(B7) -1) - 1</f>
+      <c r="C6" s="15">
+        <f>CODE(LEFT(B6,1)) -65</f>
+        <v>7</v>
+      </c>
+      <c r="D6" s="15">
+        <f>MID(B6,2,LEN(B6) -1) - 1</f>
         <v>24</v>
       </c>
-      <c r="E7" s="15">
-        <f>((D7)*25) +(C7) +1</f>
+      <c r="E6" s="15">
+        <f>((D6)*25) +(C6) +1</f>
         <v>608</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="15">
-        <f>CODE(LEFT(F7,1)) -65</f>
+      <c r="G6" s="15">
+        <f>CODE(LEFT(F6,1)) -65</f>
         <v>11</v>
       </c>
-      <c r="H7" s="15">
-        <f>MID(F7,2,LEN(F7) -1) - 1</f>
-        <v>4</v>
-      </c>
-      <c r="I7" s="15">
-        <f>((H7)*25) +(G7) +1</f>
+      <c r="H6" s="15">
+        <f>MID(F6,2,LEN(F6) -1) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="I6" s="15">
+        <f>((H6)*25) +(G6) +1</f>
         <v>112</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="15" t="str">
-        <f t="shared" ref="L7" si="5">MID(J7,2,LEN(J7) -1)</f>
+      <c r="J6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="15" t="str">
+        <f t="shared" ref="L6" si="5">MID(J6,2,LEN(J6) -1)</f>
         <v>/////</v>
       </c>
-      <c r="M7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="P7" s="15" t="str">
-        <f t="shared" ref="P7" si="6">MID(N7,2,LEN(N7) -1)</f>
+      <c r="M6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="15" t="str">
+        <f t="shared" ref="P6" si="6">MID(N6,2,LEN(N6) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Q7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="T7" s="15" t="str">
+      <c r="Q6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="U7" s="15" t="s">
+      <c r="U6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="W6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X6" s="15" t="str">
+        <f t="shared" ref="X6" si="7">MID(V6,2,LEN(V6) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="15">
+        <f>CODE(LEFT(B8,1)) -65</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="15">
+        <f>MID(B8,2,LEN(B8) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="15">
+        <f>((D8)*25) +(C8) +1</f>
         <v>80</v>
       </c>
-      <c r="V7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X7" s="15" t="str">
-        <f t="shared" ref="X7" si="7">MID(V7,2,LEN(V7) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y7" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="15">
-        <f>CODE(LEFT(B9,1)) -65</f>
-        <v>4</v>
-      </c>
-      <c r="D9" s="15">
-        <f>MID(B9,2,LEN(B9) -1) - 1</f>
-        <v>3</v>
-      </c>
-      <c r="E9" s="15">
-        <f>((D9)*25) +(C9) +1</f>
-        <v>80</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="15">
-        <f>CODE(LEFT(F9,1)) -65</f>
+      <c r="F8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="15">
+        <f>CODE(LEFT(F8,1)) -65</f>
         <v>15</v>
       </c>
-      <c r="H9" s="15">
-        <f>MID(F9,2,LEN(F9) -1) - 1</f>
-        <v>4</v>
-      </c>
-      <c r="I9" s="15">
-        <f>((H9)*25) +(G9) +1</f>
+      <c r="H8" s="15">
+        <f>MID(F8,2,LEN(F8) -1) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="I8" s="15">
+        <f>((H8)*25) +(G8) +1</f>
         <v>116</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J8" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="15">
-        <f>CODE(LEFT(J9,1)) -65</f>
+      <c r="K8" s="15">
+        <f>CODE(LEFT(J8,1)) -65</f>
         <v>17</v>
       </c>
-      <c r="L9" s="15">
-        <f>MID(J9,2,LEN(J9) -1) - 1</f>
+      <c r="L8" s="15">
+        <f>MID(J8,2,LEN(J8) -1) - 1</f>
         <v>17</v>
       </c>
-      <c r="M9" s="15">
-        <f>((L9)*25) +(K9) +1</f>
+      <c r="M8" s="15">
+        <f>((L8)*25) +(K8) +1</f>
         <v>443</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="15">
-        <f>CODE(LEFT(N9,1)) -65</f>
+      <c r="O8" s="15">
+        <f>CODE(LEFT(N8,1)) -65</f>
         <v>12</v>
       </c>
-      <c r="P9" s="15">
-        <f>MID(N9,2,LEN(N9) -1) - 1</f>
+      <c r="P8" s="15">
+        <f>MID(N8,2,LEN(N8) -1) - 1</f>
         <v>18</v>
       </c>
-      <c r="Q9" s="15">
-        <f>((P9)*25) +(O9) +1</f>
+      <c r="Q8" s="15">
+        <f>((P8)*25) +(O8) +1</f>
         <v>463</v>
       </c>
-      <c r="R9" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S9" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="T9" s="15" t="str">
+      <c r="R8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T8" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="U9" s="15" t="s">
+      <c r="U8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X8" s="15" t="str">
+        <f t="shared" ref="X8" si="8">MID(V8,2,LEN(V8) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="15">
+        <f>CODE(LEFT(B10,1)) -65</f>
+        <v>12</v>
+      </c>
+      <c r="D10" s="15">
+        <f>MID(B10,2,LEN(B10) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="E10" s="15">
+        <f>((D10)*25) +(C10) +1</f>
+        <v>488</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="V9" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W9" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X9" s="15" t="str">
-        <f t="shared" ref="X9" si="8">MID(V9,2,LEN(V9) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y9" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="15">
-        <f>CODE(LEFT(B11,1)) -65</f>
-        <v>12</v>
-      </c>
-      <c r="D11" s="15">
-        <f>MID(B11,2,LEN(B11) -1) - 1</f>
-        <v>19</v>
-      </c>
-      <c r="E11" s="15">
-        <f>((D11)*25) +(C11) +1</f>
-        <v>488</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="15">
-        <f>CODE(LEFT(F11,1)) -65</f>
+      <c r="G10" s="15">
+        <f>CODE(LEFT(F10,1)) -65</f>
         <v>15</v>
       </c>
-      <c r="H11" s="15">
-        <f>MID(F11,2,LEN(F11) -1) - 1</f>
+      <c r="H10" s="15">
+        <f>MID(F10,2,LEN(F10) -1) - 1</f>
         <v>3</v>
       </c>
-      <c r="I11" s="15">
-        <f>((H11)*25) +(G11) +1</f>
+      <c r="I10" s="15">
+        <f>((H10)*25) +(G10) +1</f>
         <v>91</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="15">
-        <f>CODE(LEFT(J11,1)) -65</f>
+      <c r="K10" s="15">
+        <f>CODE(LEFT(J10,1)) -65</f>
         <v>18</v>
       </c>
-      <c r="L11" s="15">
-        <f>MID(J11,2,LEN(J11) -1) - 1</f>
+      <c r="L10" s="15">
+        <f>MID(J10,2,LEN(J10) -1) - 1</f>
         <v>16</v>
       </c>
-      <c r="M11" s="15">
-        <f>((L11)*25) +(K11) +1</f>
+      <c r="M10" s="15">
+        <f>((L10)*25) +(K10) +1</f>
         <v>419</v>
       </c>
-      <c r="N11" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="O11" s="15">
-        <f>CODE(LEFT(N11,1)) -65</f>
+      <c r="N10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="15">
+        <f>CODE(LEFT(N10,1)) -65</f>
         <v>3</v>
       </c>
-      <c r="P11" s="15">
-        <f>MID(N11,2,LEN(N11) -1) - 1</f>
+      <c r="P10" s="15">
+        <f>MID(N10,2,LEN(N10) -1) - 1</f>
         <v>3</v>
       </c>
-      <c r="Q11" s="15">
-        <f>((P11)*25) +(O11) +1</f>
+      <c r="Q10" s="15">
+        <f>((P10)*25) +(O10) +1</f>
         <v>79</v>
       </c>
-      <c r="R11" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S11" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="T11" s="15" t="str">
+      <c r="R10" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T10" s="15" t="str">
         <f t="shared" si="2"/>
         <v>/////</v>
       </c>
-      <c r="U11" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="V11" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W11" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X11" s="15" t="str">
-        <f t="shared" ref="X11" si="9">MID(V11,2,LEN(V11) -1)</f>
+      <c r="U10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X10" s="15" t="str">
+        <f t="shared" ref="X10" si="9">MID(V10,2,LEN(V10) -1)</f>
         <v>/////</v>
       </c>
-      <c r="Y11" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="Y10" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="15">
+        <f>CODE(LEFT(B12,1)) -65</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f>MID(B12,2,LEN(B12) -1) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
+        <f>((D12)*25) +(C12) +1</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="15">
+        <f>CODE(LEFT(F12,1)) -65</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="15">
+        <f>MID(F12,2,LEN(F12) -1) - 1</f>
+        <v>12</v>
+      </c>
+      <c r="I12" s="15">
+        <f>((H12)*25) +(G12) +1</f>
+        <v>303</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="15">
+        <f>CODE(LEFT(J12,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="L12" s="15">
+        <f>MID(J12,2,LEN(J12) -1) - 1</f>
+        <v>6</v>
+      </c>
+      <c r="M12" s="15">
+        <f>((L12)*25) +(K12) +1</f>
+        <v>160</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="O12" s="15">
+        <f>CODE(LEFT(N12,1)) -65</f>
+        <v>9</v>
+      </c>
+      <c r="P12" s="15">
+        <f>MID(N12,2,LEN(N12) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="Q12" s="15">
+        <f>((P12)*25) +(O12) +1</f>
+        <v>485</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="S12" s="15">
+        <f>CODE(LEFT(R12,1)) -65</f>
+        <v>20</v>
+      </c>
+      <c r="T12" s="15">
+        <f>MID(R12,2,LEN(R12) -1) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="U12" s="15">
+        <f>((T12)*25) +(S12) +1</f>
+        <v>96</v>
+      </c>
+      <c r="V12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="W12" s="15">
+        <f>CODE(LEFT(V12,1)) -65</f>
+        <v>21</v>
+      </c>
+      <c r="X12" s="15">
+        <f>MID(V12,2,LEN(V12) -1) - 1</f>
+        <v>19</v>
+      </c>
+      <c r="Y12" s="15">
+        <f>((X12)*25) +(W12) +1</f>
+        <v>497</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="15">
-        <f>CODE(LEFT(B13,1)) -65</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="15">
-        <f>MID(B13,2,LEN(B13) -1) - 1</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="15">
-        <f>((D13)*25) +(C13) +1</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="15">
-        <f>CODE(LEFT(F13,1)) -65</f>
+      <c r="B13" s="19"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="15" t="str">
+        <f t="shared" ref="D14" si="10">MID(B14,2,LEN(B14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="15" t="str">
+        <f t="shared" ref="H14" si="11">MID(F14,2,LEN(F14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="15" t="str">
+        <f t="shared" ref="L14" si="12">MID(J14,2,LEN(J14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" s="15" t="str">
+        <f t="shared" ref="P14" si="13">MID(N14,2,LEN(N14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15" t="str">
+        <f t="shared" ref="T14" si="14">MID(R14,2,LEN(R14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X14" s="15" t="str">
+        <f t="shared" ref="X14" si="15">MID(V14,2,LEN(V14) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="15">
+        <f>CODE(LEFT(B15,1)) -65</f>
         <v>2</v>
       </c>
-      <c r="H13" s="15">
-        <f>MID(F13,2,LEN(F13) -1) - 1</f>
-        <v>12</v>
-      </c>
-      <c r="I13" s="15">
-        <f>((H13)*25) +(G13) +1</f>
-        <v>303</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="15">
-        <f>CODE(LEFT(J13,1)) -65</f>
-        <v>9</v>
-      </c>
-      <c r="L13" s="15">
-        <f>MID(J13,2,LEN(J13) -1) - 1</f>
+      <c r="D15" s="15">
+        <f>MID(B15,2,LEN(B15) -1) - 1</f>
+        <v>13</v>
+      </c>
+      <c r="E15" s="15">
+        <f>((D15)*25) +(C15) +1</f>
+        <v>328</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="15">
+        <f>CODE(LEFT(F15,1)) -65</f>
         <v>6</v>
       </c>
-      <c r="M13" s="15">
-        <f>((L13)*25) +(K13) +1</f>
-        <v>160</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="O13" s="15">
-        <f>CODE(LEFT(N13,1)) -65</f>
-        <v>9</v>
-      </c>
-      <c r="P13" s="15">
-        <f>MID(N13,2,LEN(N13) -1) - 1</f>
-        <v>19</v>
-      </c>
-      <c r="Q13" s="15">
-        <f>((P13)*25) +(O13) +1</f>
-        <v>485</v>
-      </c>
-      <c r="R13" s="19" t="s">
+      <c r="H15" s="15">
+        <f>MID(F15,2,LEN(F15) -1) - 1</f>
+        <v>13</v>
+      </c>
+      <c r="I15" s="15">
+        <f>((H15)*25) +(G15) +1</f>
+        <v>332</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="15">
+        <f>CODE(LEFT(J15,1)) -65</f>
+        <v>11</v>
+      </c>
+      <c r="L15" s="15">
+        <f>MID(J15,2,LEN(J15) -1) - 1</f>
+        <v>8</v>
+      </c>
+      <c r="M15" s="15">
+        <f>((L15)*25) +(K15) +1</f>
+        <v>212</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="15">
+        <f>CODE(LEFT(N15,1)) -65</f>
+        <v>10</v>
+      </c>
+      <c r="P15" s="15">
+        <f>MID(N15,2,LEN(N15) -1) - 1</f>
+        <v>8</v>
+      </c>
+      <c r="Q15" s="15">
+        <f>((P15)*25) +(O15) +1</f>
+        <v>211</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="T15" s="15" t="str">
+        <f t="shared" ref="S15:T15" si="16">MID(R15,2,LEN(R15) -1)</f>
+        <v>/////</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V15" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="W15" s="15">
+        <f>CODE(LEFT(V15,1)) -65</f>
+        <v>22</v>
+      </c>
+      <c r="X15" s="15">
+        <f>MID(V15,2,LEN(V15) -1) - 1</f>
+        <v>24</v>
+      </c>
+      <c r="Y15" s="15">
+        <f>((X15)*25) +(W15) +1</f>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="S13" s="15">
-        <f>CODE(LEFT(R13,1)) -65</f>
-        <v>20</v>
-      </c>
-      <c r="T13" s="15">
-        <f>MID(R13,2,LEN(R13) -1) - 1</f>
-        <v>3</v>
-      </c>
-      <c r="U13" s="15">
-        <f>((T13)*25) +(S13) +1</f>
-        <v>96</v>
-      </c>
-      <c r="V13" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="W13" s="15">
-        <f>CODE(LEFT(V13,1)) -65</f>
-        <v>21</v>
-      </c>
-      <c r="X13" s="15">
-        <f>MID(V13,2,LEN(V13) -1) - 1</f>
-        <v>19</v>
-      </c>
-      <c r="Y13" s="15">
-        <f>((X13)*25) +(W13) +1</f>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="15" t="str">
-        <f t="shared" ref="D15" si="10">MID(B15,2,LEN(B15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="15" t="str">
-        <f t="shared" ref="H15" si="11">MID(F15,2,LEN(F15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="15" t="str">
-        <f t="shared" ref="L15" si="12">MID(J15,2,LEN(J15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="P15" s="15" t="str">
-        <f t="shared" ref="P15" si="13">MID(N15,2,LEN(N15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15" t="str">
-        <f t="shared" ref="T15" si="14">MID(R15,2,LEN(R15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="U15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="V15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X15" s="15" t="str">
-        <f t="shared" ref="X15" si="15">MID(V15,2,LEN(V15) -1)</f>
-        <v>/////</v>
-      </c>
-      <c r="Y15" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>63</v>
       </c>
       <c r="C16" s="15">
         <f>CODE(LEFT(B16,1)) -65</f>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D16" s="15">
         <f>MID(B16,2,LEN(B16) -1) - 1</f>
@@ -4304,83 +4387,39 @@
       </c>
       <c r="E16" s="15">
         <f>((D16)*25) +(C16) +1</f>
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G16" s="15">
         <f>CODE(LEFT(F16,1)) -65</f>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H16" s="15">
         <f>MID(F16,2,LEN(F16) -1) - 1</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I16" s="15">
         <f>((H16)*25) +(G16) +1</f>
-        <v>212</v>
-      </c>
-      <c r="J16" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="15">
-        <f>CODE(LEFT(J16,1)) -65</f>
-        <v>17</v>
-      </c>
-      <c r="L16" s="15">
-        <f>MID(J16,2,LEN(J16) -1) - 1</f>
-        <v>23</v>
-      </c>
-      <c r="M16" s="15">
-        <f>((L16)*25) +(K16) +1</f>
-        <v>593</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="O16" s="15">
-        <f>CODE(LEFT(N16,1)) -65</f>
-        <v>10</v>
-      </c>
-      <c r="P16" s="15">
-        <f>MID(N16,2,LEN(N16) -1) - 1</f>
-        <v>8</v>
-      </c>
-      <c r="Q16" s="15">
-        <f>((P16)*25) +(O16) +1</f>
-        <v>211</v>
-      </c>
-      <c r="R16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="S16" s="15">
-        <f>CODE(LEFT(R16,1)) -65</f>
-        <v>6</v>
-      </c>
-      <c r="T16" s="15">
-        <f>MID(R16,2,LEN(R16) -1) - 1</f>
-        <v>13</v>
-      </c>
-      <c r="U16" s="15">
-        <f>((T16)*25) +(S16) +1</f>
-        <v>332</v>
-      </c>
-      <c r="V16" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="W16" s="15">
-        <f>CODE(LEFT(V16,1)) -65</f>
-        <v>22</v>
-      </c>
-      <c r="X16" s="15">
-        <f>MID(V16,2,LEN(V16) -1) - 1</f>
-        <v>24</v>
-      </c>
-      <c r="Y16" s="15">
-        <f>((X16)*25) +(W16) +1</f>
-        <v>623</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="J16" s="19"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
@@ -4473,54 +4512,54 @@
         <v>463</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T18" s="15" t="str">
-        <f t="shared" ref="T18" si="16">MID(R18,2,LEN(R18) -1)</f>
+        <f t="shared" ref="T18" si="17">MID(R18,2,LEN(R18) -1)</f>
         <v>/////</v>
       </c>
       <c r="U18" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="V18" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W18" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="X18" s="15" t="str">
-        <f t="shared" ref="X18" si="17">MID(V18,2,LEN(V18) -1)</f>
+        <f t="shared" ref="X18" si="18">MID(V18,2,LEN(V18) -1)</f>
         <v>/////</v>
       </c>
       <c r="Y18" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="D22" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="14">
         <f>CODE(LEFT(B23,1)) -65</f>
@@ -4535,9 +4574,14 @@
         <v>303</v>
       </c>
     </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -4545,7 +4589,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D27">
         <v>25</v>
@@ -4553,26 +4597,26 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="D30" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="14">
         <f>CODE(LEFT(B31,1)) -65</f>
@@ -4583,17 +4627,13 @@
         <v>0</v>
       </c>
       <c r="E31" s="17">
-        <f>((D31)*D35) +(C31) + 1</f>
+        <f>((D31)*D36) +(C31) + 1</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="H15 D15 L15 L7 P9 T16 X16 P5 L5 P7" formula="1"/>
-    <ignoredError sqref="E31" emptyCellReference="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Got rid of errors, edited calcTargets to make a list of board cells
</commit_message>
<xml_diff>
--- a/Layout/Layout.xlsx
+++ b/Layout/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15600" activeTab="1"/>
+    <workbookView xWindow="14355" yWindow="0" windowWidth="14355" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="95">
   <si>
     <t>X</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>//////////</t>
+  </si>
+  <si>
+    <t>White: Target Tests</t>
+  </si>
+  <si>
+    <t>Purple:Exit room target tests</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,12 +3395,12 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3412,7 +3418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
@@ -4351,7 +4357,7 @@
         <v>92</v>
       </c>
       <c r="T15" s="15" t="str">
-        <f t="shared" ref="S15:T15" si="16">MID(R15,2,LEN(R15) -1)</f>
+        <f t="shared" ref="T15" si="16">MID(R15,2,LEN(R15) -1)</f>
         <v>/////</v>
       </c>
       <c r="U15" s="15" t="s">

</xml_diff>